<commit_message>
improved input parameters and sample data
</commit_message>
<xml_diff>
--- a/transformations.xlsx
+++ b/transformations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualStudioCode\xlsx2transformations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code\xlsx2transformations\xlsx2transformations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17814B91-3D2C-4201-B879-2604F4FA5C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D72414-EA69-4345-830B-4C1ACA2C42B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{68011ABC-3087-43E0-A353-09322C07EED8}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21000" activeTab="1" xr2:uid="{68011ABC-3087-43E0-A353-09322C07EED8}"/>
   </bookViews>
   <sheets>
     <sheet name="agency.txt" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>op</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>https://test.de</t>
+  </si>
+  <si>
+    <t>route_url</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1681CA17-1F0C-406B-B0B8-89B399615240}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -549,10 +552,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D032EE-8369-4636-A561-75157E1A4115}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,9 +563,10 @@
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,13 +583,16 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -601,10 +608,10 @@
       <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>